<commit_message>
culture_collection を MIGS.ba etc に追加 r6369-1
</commit_message>
<xml_diff>
--- a/ykodama/ddbj_packages/excel/MIGS.ba.4.0.xlsx
+++ b/ykodama/ddbj_packages/excel/MIGS.ba.4.0.xlsx
@@ -249,11 +249,24 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>Name of source institute and unique culture identifier. See the description for the proper format and list of allowed institutes, http://www.insdc.org/controlled-vocabulary-culturecollection-qualifier</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S15" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>Traits like antibiotic resistance/xenobiotic degration phenotypes/converting phage genes</t>
         </r>
       </text>
     </comment>
-    <comment ref="S15" authorId="0">
+    <comment ref="T15" authorId="0">
       <text>
         <r>
           <rPr>
@@ -266,7 +279,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T15" authorId="0">
+    <comment ref="U15" authorId="0">
       <text>
         <r>
           <rPr>
@@ -279,7 +292,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U15" authorId="0">
+    <comment ref="V15" authorId="0">
       <text>
         <r>
           <rPr>
@@ -292,7 +305,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V15" authorId="0">
+    <comment ref="W15" authorId="0">
       <text>
         <r>
           <rPr>
@@ -305,7 +318,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W15" authorId="0">
+    <comment ref="X15" authorId="0">
       <text>
         <r>
           <rPr>
@@ -318,7 +331,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X15" authorId="0">
+    <comment ref="Y15" authorId="0">
       <text>
         <r>
           <rPr>
@@ -331,7 +344,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y15" authorId="0">
+    <comment ref="Z15" authorId="0">
       <text>
         <r>
           <rPr>
@@ -344,7 +357,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z15" authorId="0">
+    <comment ref="AA15" authorId="0">
       <text>
         <r>
           <rPr>
@@ -357,7 +370,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA15" authorId="0">
+    <comment ref="AB15" authorId="0">
       <text>
         <r>
           <rPr>
@@ -370,7 +383,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB15" authorId="0">
+    <comment ref="AC15" authorId="0">
       <text>
         <r>
           <rPr>
@@ -383,7 +396,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC15" authorId="0">
+    <comment ref="AD15" authorId="0">
       <text>
         <r>
           <rPr>
@@ -396,7 +409,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD15" authorId="0">
+    <comment ref="AE15" authorId="0">
       <text>
         <r>
           <rPr>
@@ -409,7 +422,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE15" authorId="0">
+    <comment ref="AF15" authorId="0">
       <text>
         <r>
           <rPr>
@@ -422,7 +435,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF15" authorId="0">
+    <comment ref="AG15" authorId="0">
       <text>
         <r>
           <rPr>
@@ -435,7 +448,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG15" authorId="0">
+    <comment ref="AH15" authorId="0">
       <text>
         <r>
           <rPr>
@@ -453,7 +466,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t xml:space="preserve"># This is a submission template for batch deposit of 'MIGS: cultured bacteria/archaea; version 4.0' samples to the DDBJ BioSample database (http://trace.ddbj.nig.ac.jp/biosample)._x000D_
 </t>
@@ -560,6 +573,9 @@
   </si>
   <si>
     <t>biotic_relationship</t>
+  </si>
+  <si>
+    <t>culture_collection</t>
   </si>
   <si>
     <t>encoded_traits</t>
@@ -1025,77 +1041,77 @@
     <col min="1" max="201" width="20.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33">
+    <row r="1" spans="1:34">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:33">
+    <row r="2" spans="1:34">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:33" s="3" customFormat="1">
+    <row r="3" spans="1:34" s="3" customFormat="1">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:33" s="4" customFormat="1">
+    <row r="4" spans="1:34" s="4" customFormat="1">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:33" s="5" customFormat="1">
+    <row r="5" spans="1:34" s="5" customFormat="1">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:33">
+    <row r="6" spans="1:34">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:33">
+    <row r="7" spans="1:34">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:33">
+    <row r="8" spans="1:34">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:33">
+    <row r="9" spans="1:34">
       <c r="A9" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:33">
+    <row r="10" spans="1:34">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:33">
+    <row r="11" spans="1:34">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:33">
+    <row r="12" spans="1:34">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:33">
+    <row r="13" spans="1:34">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:33">
+    <row r="14" spans="1:34">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:33">
+    <row r="15" spans="1:34">
       <c r="A15" s="7" t="s">
         <v>14</v>
       </c>
@@ -1194,6 +1210,9 @@
       </c>
       <c r="AG15" s="8" t="s">
         <v>46</v>
+      </c>
+      <c r="AH15" s="8" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
culture collection を MIxS から再度削除 INSDC2017 での確認に基づく
</commit_message>
<xml_diff>
--- a/ykodama/ddbj_packages/excel/MIGS.ba.4.0.xlsx
+++ b/ykodama/ddbj_packages/excel/MIGS.ba.4.0.xlsx
@@ -249,7 +249,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Name of source institute and unique culture identifier. See the description for the proper format and list of allowed institutes, http://www.insdc.org/controlled-vocabulary-culturecollection-qualifier</t>
+          <t>Traits like antibiotic resistance/xenobiotic degration phenotypes/converting phage genes</t>
         </r>
       </text>
     </comment>
@@ -262,7 +262,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Traits like antibiotic resistance/xenobiotic degration phenotypes/converting phage genes</t>
+          <t>Estimated size of genome</t>
         </r>
       </text>
     </comment>
@@ -275,7 +275,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Estimated size of genome</t>
+          <t>Plasmids that have significance phenotypic consequence</t>
         </r>
       </text>
     </comment>
@@ -288,7 +288,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Plasmids that have significance phenotypic consequence</t>
+          <t>Health or disease status of sample at time of collection</t>
         </r>
       </text>
     </comment>
@@ -301,7 +301,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Health or disease status of sample at time of collection</t>
+          <t>The natural (as opposed to laboratory) host to the organism from which the sample was obtained. Use the full taxonomic name, eg, "Homo sapiens".</t>
         </r>
       </text>
     </comment>
@@ -314,7 +314,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The natural (as opposed to laboratory) host to the organism from which the sample was obtained. Use the full taxonomic name, eg, "Homo sapiens".</t>
+          <t>NCBI taxonomy ID of the host, e.g. 9606</t>
         </r>
       </text>
     </comment>
@@ -327,7 +327,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>NCBI taxonomy ID of the host, e.g. 9606</t>
+          <t>Describes the physical, environmental and/or local geographical source of the biological sample from which the sample was derived.</t>
         </r>
       </text>
     </comment>
@@ -340,7 +340,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Describes the physical, environmental and/or local geographical source of the biological sample from which the sample was derived.</t>
+          <t>A locus tag prefix required for an annotated genome, http://www.ddbj.nig.ac.jp/sub/locus_tag-e.html</t>
         </r>
       </text>
     </comment>
@@ -353,7 +353,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>A locus tag prefix required for an annotated genome, http://www.ddbj.nig.ac.jp/sub/locus_tag-e.html</t>
+          <t>To what is the entity pathogenic</t>
         </r>
       </text>
     </comment>
@@ -366,7 +366,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>To what is the entity pathogenic</t>
+          <t>Aerobic or anaerobic</t>
         </r>
       </text>
     </comment>
@@ -379,7 +379,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Aerobic or anaerobic</t>
+          <t>Method or device employed for collecting sample</t>
         </r>
       </text>
     </comment>
@@ -392,7 +392,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Method or device employed for collecting sample</t>
+          <t>Processing applied to the sample during or after isolation</t>
         </r>
       </text>
     </comment>
@@ -405,7 +405,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Processing applied to the sample during or after isolation</t>
+          <t>Amount or size of sample (volume, mass or area) that was collected</t>
         </r>
       </text>
     </comment>
@@ -418,7 +418,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Amount or size of sample (volume, mass or area) that was collected</t>
+          <t>unique identifier assigned to a material sample used for extracting nucleic acids, and subsequent sequencing. The identifier can refer either to the original material collected or to any derived sub-samples.</t>
         </r>
       </text>
     </comment>
@@ -431,24 +431,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>unique identifier assigned to a material sample used for extracting nucleic acids, and subsequent sequencing. The identifier can refer either to the original material collected or to any derived sub-samples.</t>
+          <t>Information about the genetic distinctness of the lineage (eg., biovar, serovar)</t>
         </r>
       </text>
     </comment>
     <comment ref="AG15" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Information about the genetic distinctness of the lineage (eg., biovar, serovar)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AH15" authorId="0">
       <text>
         <r>
           <rPr>
@@ -466,7 +453,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t xml:space="preserve"># This is a submission template for batch deposit of 'MIGS: cultured bacteria/archaea; version 4.0' samples to the DDBJ BioSample database (http://trace.ddbj.nig.ac.jp/biosample)._x000D_
 </t>
@@ -573,9 +560,6 @@
   </si>
   <si>
     <t>biotic_relationship</t>
-  </si>
-  <si>
-    <t>culture_collection</t>
   </si>
   <si>
     <t>encoded_traits</t>
@@ -1041,77 +1025,77 @@
     <col min="1" max="201" width="20.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:33">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:34">
+    <row r="2" spans="1:33">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:34" s="3" customFormat="1">
+    <row r="3" spans="1:33" s="3" customFormat="1">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:34" s="4" customFormat="1">
+    <row r="4" spans="1:33" s="4" customFormat="1">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:34" s="5" customFormat="1">
+    <row r="5" spans="1:33" s="5" customFormat="1">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:34">
+    <row r="6" spans="1:33">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:34">
+    <row r="7" spans="1:33">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:34">
+    <row r="8" spans="1:33">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:34">
+    <row r="9" spans="1:33">
       <c r="A9" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:34">
+    <row r="10" spans="1:33">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:34">
+    <row r="11" spans="1:33">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:34">
+    <row r="12" spans="1:33">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:34">
+    <row r="13" spans="1:33">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:34">
+    <row r="14" spans="1:33">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:34">
+    <row r="15" spans="1:33">
       <c r="A15" s="7" t="s">
         <v>14</v>
       </c>
@@ -1210,9 +1194,6 @@
       </c>
       <c r="AG15" s="8" t="s">
         <v>46</v>
-      </c>
-      <c r="AH15" s="8" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>